<commit_message>
Add ExcelMapperOptions; Refactor AnnotationBasedExcelMappingDriver; Add formaters
</commit_message>
<xml_diff>
--- a/sample/sample.xlsx
+++ b/sample/sample.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\env\Code\java\my\excel\excel\sample\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\env\Code\java\my\excel-mapper\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Колонка long</t>
   </si>
@@ -32,6 +32,18 @@
   </si>
   <si>
     <t>Колонка после пропуска с датой</t>
+  </si>
+  <si>
+    <t>ab</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
   </si>
 </sst>
 </file>
@@ -302,17 +314,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A2:E1000"/>
+  <dimension ref="A2:F1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="27" customWidth="1"/>
     <col min="5" max="5" width="34.42578125" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -325,8 +340,11 @@
       <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" s="3">
+        <v>45209</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -342,8 +360,11 @@
       <c r="E3" s="3">
         <v>45209</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -357,8 +378,11 @@
       <c r="E4" s="3">
         <v>20000</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -374,8 +398,11 @@
       <c r="E5" s="3">
         <v>30000</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="2">
         <v>40</v>
@@ -389,8 +416,11 @@
       <c r="E6" s="3">
         <v>40000</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -407,7 +437,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B8" s="2">
         <v>602436346346.33496</v>
       </c>
@@ -416,28 +446,28 @@
       </c>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E14" s="4"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E16" s="4"/>
     </row>
     <row r="17" spans="5:5" x14ac:dyDescent="0.2">

</xml_diff>